<commit_message>
nije jos gotovo, sajt nije radio kad sam ja mogao da radim, pa nije jos skroz gotovo, doradicu jos
</commit_message>
<xml_diff>
--- a/data/testCases.xlsx
+++ b/data/testCases.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1Strahinja1\programming\workspace\SeleniumProject\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Strahinja\Desktop\SeleniumWorkspace\FinalProjectSelenium\SeleniumProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F22EB2-8968-4203-9272-32B786B88161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CDAC85-3B32-45E6-9830-8D72B8B2DCAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13395" yWindow="1140" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC1-MyInfo" sheetId="5" r:id="rId1"/>
     <sheet name="TC2-Address" sheetId="3" r:id="rId2"/>
-    <sheet name="TC4-PersonalInformation" sheetId="6" r:id="rId3"/>
-    <sheet name="TC3-Login" sheetId="4" r:id="rId4"/>
+    <sheet name="TC3-Login" sheetId="4" r:id="rId3"/>
+    <sheet name="TC4-PersonalInformation" sheetId="6" r:id="rId4"/>
+    <sheet name="TC5-MyWishList" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="92">
   <si>
     <t>same</t>
   </si>
@@ -171,21 +172,6 @@
     <t>input value</t>
   </si>
   <si>
-    <t>Strahinja</t>
-  </si>
-  <si>
-    <t>Jelic</t>
-  </si>
-  <si>
-    <t>Samsung</t>
-  </si>
-  <si>
-    <t>Gunduliceva 5</t>
-  </si>
-  <si>
-    <t>Gunduliceva 6</t>
-  </si>
-  <si>
     <t>Beograd</t>
   </si>
   <si>
@@ -229,6 +215,105 @@
   </si>
   <si>
     <t>actual resault</t>
+  </si>
+  <si>
+    <t>TestCase id</t>
+  </si>
+  <si>
+    <t>test case name</t>
+  </si>
+  <si>
+    <t>changing personal info</t>
+  </si>
+  <si>
+    <t>click on 'MY PERSONAL INFORMATION'  btn</t>
+  </si>
+  <si>
+    <t>page with personal value loaded</t>
+  </si>
+  <si>
+    <t>Chose "Mrs." checkbox</t>
+  </si>
+  <si>
+    <t>insert 'First name'</t>
+  </si>
+  <si>
+    <t>Ivana</t>
+  </si>
+  <si>
+    <t>insert 'Last name'</t>
+  </si>
+  <si>
+    <t>Ivanovic</t>
+  </si>
+  <si>
+    <t>insert 'E-mail address'</t>
+  </si>
+  <si>
+    <t>ivanaivanovictest@gmail.com</t>
+  </si>
+  <si>
+    <t>chose "1" from drpdwn box day</t>
+  </si>
+  <si>
+    <t>chose "January" from month box</t>
+  </si>
+  <si>
+    <t>choose "2000" from year box</t>
+  </si>
+  <si>
+    <t>insert 'Current Password'</t>
+  </si>
+  <si>
+    <t>insert 'New Password'</t>
+  </si>
+  <si>
+    <t>Strahinja2.</t>
+  </si>
+  <si>
+    <t>insert 'Confirmation'</t>
+  </si>
+  <si>
+    <t>click 'Save &gt;' btn</t>
+  </si>
+  <si>
+    <t>click 'OK' on alert window</t>
+  </si>
+  <si>
+    <t>Aleksa</t>
+  </si>
+  <si>
+    <t>Obradovic</t>
+  </si>
+  <si>
+    <t>Arsenija Carnojevica 5</t>
+  </si>
+  <si>
+    <t>Arsenija Carnojevica 5a</t>
+  </si>
+  <si>
+    <t>ARSENIJA CARNOJEVICA</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>assert</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>21000</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Wish list name</t>
+  </si>
+  <si>
+    <t>Strahinja Jelic</t>
   </si>
 </sst>
 </file>
@@ -281,7 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -297,6 +382,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -581,18 +677,18 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="A2:D7"/>
+      <selection activeCell="D12" sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -606,12 +702,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -622,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -630,7 +726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -638,7 +734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -659,22 +755,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B80B7B-858D-4D04-8B94-323429EADD60}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection sqref="A1:G44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -682,7 +778,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -693,13 +789,16 @@
         <v>43</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -707,119 +806,122 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="C12">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="C13">
-        <v>21654321</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="C14">
-        <v>63654321</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -827,7 +929,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -838,13 +940,13 @@
         <v>43</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -852,119 +954,119 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="7">
         <v>21000</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>36</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E35" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -972,7 +1074,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>19</v>
       </c>
@@ -983,13 +1085,13 @@
         <v>43</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -997,17 +1099,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>42</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E41" t="s">
         <v>0</v>
@@ -1015,22 +1117,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F412522C-9B60-4921-AC4B-78AC4082F81A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8B4DF1-63E9-45B5-9F6C-30CEEC6585EB}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -1038,15 +1129,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1061,12 +1152,12 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1077,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1085,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1093,7 +1184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1104,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1118,12 +1209,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1134,7 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1142,7 +1233,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1150,7 +1241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1161,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1175,12 +1266,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1191,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1199,7 +1290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1207,7 +1298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1218,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
@@ -1232,12 +1323,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1248,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1257,7 +1348,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1266,7 +1357,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1286,4 +1377,227 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F412522C-9B60-4921-AC4B-78AC4082F81A}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="9">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="9">
+        <v>2000</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{8DA48B5C-BA39-4DEC-A014-B0522B8C6849}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30C475-B9CF-4BD9-BF19-5822207F03BD}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>